<commit_message>
Update Matiz de Pruebas SIEDNL - Ficha Técnica.xlsx
Actualización de archivo
</commit_message>
<xml_diff>
--- a/SIEDNL (PDR)/ENTREGABLES/Matriz de Pruebas/Matiz de Pruebas SIEDNL - Ficha Técnica.xlsx
+++ b/SIEDNL (PDR)/ENTREGABLES/Matriz de Pruebas/Matiz de Pruebas SIEDNL - Ficha Técnica.xlsx
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="174">
   <si>
     <t xml:space="preserve">Tester: Iris Lechuga </t>
   </si>
@@ -632,6 +632,9 @@
   </si>
   <si>
     <t>Marlon Israel Mendez</t>
+  </si>
+  <si>
+    <t>https://siednl.atlassian.net/browse/PBR-46</t>
   </si>
 </sst>
 </file>
@@ -1003,6 +1006,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1052,9 +1058,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9872,128 +9875,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
-  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Cuenta de N° Caso" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="5">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A47:B49" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
@@ -10171,7 +10052,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
   <location ref="A24:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
@@ -10223,6 +10104,128 @@
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Cuenta de N° Caso" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -10511,9 +10514,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:N283"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M33" sqref="M33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -10535,94 +10538,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
     </row>
     <row r="3" spans="1:14" s="20" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="31" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
     </row>
     <row r="4" spans="1:14" s="20" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
     </row>
     <row r="5" spans="1:14" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="39" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
     </row>
     <row r="6" spans="1:14" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
@@ -10957,6 +10960,9 @@
       <c r="J16" s="26" t="s">
         <v>171</v>
       </c>
+      <c r="M16" t="s">
+        <v>173</v>
+      </c>
       <c r="N16" s="1">
         <v>45097</v>
       </c>
@@ -10992,6 +10998,9 @@
       <c r="J17" s="26" t="s">
         <v>171</v>
       </c>
+      <c r="M17" t="s">
+        <v>173</v>
+      </c>
       <c r="N17" s="1">
         <v>45097</v>
       </c>
@@ -11027,6 +11036,9 @@
       <c r="J18" s="26" t="s">
         <v>171</v>
       </c>
+      <c r="M18" t="s">
+        <v>173</v>
+      </c>
       <c r="N18" s="1">
         <v>45097</v>
       </c>
@@ -11509,8 +11521,11 @@
       <c r="I34" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="J34" s="44" t="s">
+      <c r="J34" s="27" t="s">
         <v>171</v>
+      </c>
+      <c r="M34" t="s">
+        <v>173</v>
       </c>
       <c r="N34" s="1">
         <v>45097</v>
@@ -11544,8 +11559,11 @@
       <c r="I35" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J35" s="44" t="s">
+      <c r="J35" s="27" t="s">
         <v>171</v>
+      </c>
+      <c r="M35" t="s">
+        <v>173</v>
       </c>
       <c r="N35" s="1">
         <v>45097</v>
@@ -11579,8 +11597,11 @@
       <c r="I36" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J36" s="44" t="s">
+      <c r="J36" s="27" t="s">
         <v>171</v>
+      </c>
+      <c r="M36" t="s">
+        <v>173</v>
       </c>
       <c r="N36" s="1">
         <v>45097</v>
@@ -11869,8 +11890,11 @@
       <c r="I46" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J46" s="44" t="s">
+      <c r="J46" s="27" t="s">
         <v>171</v>
+      </c>
+      <c r="M46" t="s">
+        <v>173</v>
       </c>
       <c r="N46" s="1">
         <v>45097</v>
@@ -12082,8 +12106,11 @@
       <c r="I53" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="J53" s="44" t="s">
+      <c r="J53" s="27" t="s">
         <v>171</v>
+      </c>
+      <c r="M53" t="s">
+        <v>173</v>
       </c>
       <c r="N53" s="1">
         <v>45097</v>
@@ -12117,8 +12144,11 @@
       <c r="I54" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J54" s="44" t="s">
+      <c r="J54" s="27" t="s">
         <v>171</v>
+      </c>
+      <c r="M54" t="s">
+        <v>173</v>
       </c>
       <c r="N54" s="1">
         <v>45097</v>
@@ -12152,8 +12182,11 @@
       <c r="I55" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J55" s="44" t="s">
+      <c r="J55" s="27" t="s">
         <v>171</v>
+      </c>
+      <c r="M55" t="s">
+        <v>173</v>
       </c>
       <c r="N55" s="1">
         <v>45097</v>

</xml_diff>